<commit_message>
✨ Add "Exemplaires" link to games on game page
</commit_message>
<xml_diff>
--- a/backlog/ProductBacklog.xlsx
+++ b/backlog/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcornuault2022\eclipse-workspace\ludotheque\backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F43401-EEF3-4E85-A446-7FE3AE70534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6717F0-EAA9-4DDB-851E-E9E179B005B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
@@ -690,7 +690,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +875,7 @@
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
✨ Add "Exemplaires" modifying
</commit_message>
<xml_diff>
--- a/backlog/ProductBacklog.xlsx
+++ b/backlog/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcornuault2022\eclipse-workspace\ludotheque\backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6717F0-EAA9-4DDB-851E-E9E179B005B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE79132-65A8-4318-BFEF-DFBF0486B772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
@@ -690,7 +690,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
🔨 Update product backlog
</commit_message>
<xml_diff>
--- a/backlog/ProductBacklog.xlsx
+++ b/backlog/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcornuault2022\eclipse-workspace\ludotheque\backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE79132-65A8-4318-BFEF-DFBF0486B772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10C32CC-97A3-4ACC-95F9-B8ED05D937E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>PRODUCT BACKLOG LUDOTHEQUE</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Mise en place SpringSecurity (build.gradle/WebSecurityConfig)</t>
+  </si>
+  <si>
+    <t>=&gt; Insert mis en place avant la consigne, Finalement je met plutôt le DELETE de jeu et ses exemplaires en proc stoc</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,6 +335,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -690,7 +696,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>2770</v>
       </c>
@@ -888,9 +894,11 @@
       <c r="C14" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="E14" s="17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,7 +911,7 @@
       <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="17" t="b">

</xml_diff>

<commit_message>
✨ Add login system with Spring Security (W.I.P 🚧)
</commit_message>
<xml_diff>
--- a/backlog/ProductBacklog.xlsx
+++ b/backlog/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcornuault2022\eclipse-workspace\ludotheque\backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10C32CC-97A3-4ACC-95F9-B8ED05D937E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E1D735-09FC-46D9-A6A5-B0CAA0522595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,9 +337,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -695,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D07A81-0E55-45DE-A090-3CCE23AAB227}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -911,11 +908,11 @@
       <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -930,7 +927,7 @@
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1109,15 +1106,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF6F188C2765874D8D7AA4700AA75D6C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2816c7b8f63b74613fdbb8b7aa2fdd36">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29b881bf-f476-448a-b14d-5abfbd8a134d" xmlns:ns3="3dc7cda2-519e-43ce-87db-fa6107af41aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf3a814e13e0688236c4fa694e00c317" ns2:_="" ns3:_="">
     <xsd:import namespace="29b881bf-f476-448a-b14d-5abfbd8a134d"/>
@@ -1318,6 +1306,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2EC614D-031B-40C4-94BE-44D07FE0C091}">
   <ds:schemaRefs>
@@ -1330,14 +1327,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97271CCD-37D0-49CB-8420-C4D5FD94F368}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D885257-0DC7-4F98-A2E3-BFF8E5B4C7BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1354,4 +1343,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97271CCD-37D0-49CB-8420-C4D5FD94F368}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
🔨 Revamp of HTML templates -> files have same "base html" index.html now
</commit_message>
<xml_diff>
--- a/backlog/ProductBacklog.xlsx
+++ b/backlog/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcornuault2022\eclipse-workspace\ludotheque\backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3738B0-E4DF-4465-8275-BDBA5A8AFAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76070884-AF2F-4D77-8E39-5850A8342128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>PRODUCT BACKLOG LUDOTHEQUE</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>=&gt; Insert mis en place avant la consigne, Finalement je met plutôt le DELETE de jeu et ses exemplaires en proc stoc</t>
+  </si>
+  <si>
+    <t>US019</t>
+  </si>
+  <si>
+    <t>Mettre en place des logs</t>
   </si>
 </sst>
 </file>
@@ -217,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +239,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,7 +355,23 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -327,11 +379,77 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D07A81-0E55-45DE-A090-3CCE23AAB227}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,10 +1000,10 @@
       <c r="B14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="17" t="b">
@@ -925,99 +1043,109 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="20">
         <v>1679</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="18" t="b">
+      <c r="D17" s="23"/>
+      <c r="E17" s="24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="20">
         <v>1599</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="18" t="b">
+      <c r="D18" s="23"/>
+      <c r="E18" s="24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="20">
         <v>1589</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="18" t="b">
+      <c r="D19" s="23"/>
+      <c r="E19" s="24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="25">
+        <v>1579</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="30">
         <v>930</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="18" t="b">
+      <c r="D21" s="33"/>
+      <c r="E21" s="34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="22" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35">
         <v>920</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="18" t="b">
+      <c r="D22" s="38"/>
+      <c r="E22" s="39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="23" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
         <v>910</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="2"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1061,11 +1189,18 @@
       <c r="D29" s="5"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="2"/>
+    </row>
     <row r="31" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D22">
-    <sortCondition descending="1" ref="A4:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D23">
+    <sortCondition descending="1" ref="A4:A23"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>